<commit_message>
I reUpload file Week_7 for laboratory 7 last time i was not able to create third task now i find solution
</commit_message>
<xml_diff>
--- a/Week_7/placeScrapy.xlsx
+++ b/Week_7/placeScrapy.xlsx
@@ -471,32 +471,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>390000₾</t>
+          <t>1210004₾</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>130 კვ.მ.</t>
+          <t>29 კვ.მ.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>13/13</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>თბილისი, დიდუბე-ჩუღურეთი, ჩუღურეთი, ი.ჯავახიშვილის ქ.</t>
+          <t>თბილისი, ვაკე-საბურთალო, ვაკე, ყიფშიძის ქ.</t>
         </is>
       </c>
     </row>
@@ -506,17 +506,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1730004₾</t>
+          <t>292000₾</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>38 კვ.მ.</t>
+          <t>97 კვ.მ.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>4/8</t>
+          <t>7/8</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -526,12 +526,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>82</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>თბილისი, ვაკე-საბურთალო, საბურთალო, ბუდაპეშტის ქ.</t>
+          <t>თბილისი, დიდუბე-ჩუღურეთი, დიდუბე, ა. წერეთლის გამზ.</t>
         </is>
       </c>
     </row>
@@ -541,32 +541,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>7400004₾</t>
+          <t>390000₾</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>150 კვ.მ.</t>
+          <t>130 კვ.მ.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1/4</t>
+          <t>2/2</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>თბილისი, ვაკე-საბურთალო, ვაკე, ფალიაშვილის ქ.</t>
+          <t>თბილისი, დიდუბე-ჩუღურეთი, ჩუღურეთი, ი.ჯავახიშვილის ქ.</t>
         </is>
       </c>
     </row>
@@ -576,12 +576,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1220003₾</t>
+          <t>5800924₾</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>38 კვ.მ.</t>
+          <t>130 კვ.მ.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -591,17 +591,17 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>4/22</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>თბილისი, გლდანი-ნაძალადევი, ნაძალადევი, ჭყონდიდელის ქ.</t>
+          <t>3/17</t>
         </is>
       </c>
     </row>
@@ -611,32 +611,32 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2330003₾</t>
+          <t>4165872₾</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>70 კვ.მ.</t>
+          <t>193 კვ.მ.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>7/14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>თბილისი, ჩაჩუა ზ. მე-2 შესახვევი 19.17 შინდისელი გმირის ქუჩა</t>
+          <t>10/11</t>
         </is>
       </c>
     </row>
@@ -646,32 +646,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2460004₾</t>
+          <t>3912252₾</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>52 კვ.მ.</t>
+          <t>150 კვ.მ.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>6/12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>2/3</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>თბილისი, ვაკე-საბურთალო, ვაკე, ნ. ჟვანიას ქ.</t>
+          <t>თბილისი, ვაკე-საბურთალო, ვაკე, მცხეთის ქ.</t>
         </is>
       </c>
     </row>
@@ -681,32 +681,32 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1300001₾</t>
+          <t>148500₾</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>87 კვ.მ.</t>
+          <t>37 კვ.მ.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2/5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>3/12</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>თბილისი, გლდანი-ნაძალადევი, ავჭალა, ლიბანის ქ.</t>
+          <t>თბილისი, ძველი თბილისი, კრწანისი, გორგასლის ქ.</t>
         </is>
       </c>
     </row>
@@ -716,32 +716,32 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>276028₾</t>
+          <t>513000₾</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>99 კვ.მ.</t>
+          <t>200 კვ.მ.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>13/16</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>თბილისი, გლდანი-ნაძალადევი, სან. ზონა, გურამიშვილის გამზ.</t>
+          <t>2/9</t>
         </is>
       </c>
     </row>
@@ -751,32 +751,32 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1960005₾</t>
+          <t>442000₾</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>38 კვ.მ.</t>
+          <t>95 კვ.მ.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>7/8</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>3/4</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>თბილისი, პეკინის ქ.</t>
+          <t>თბილისი, ვაკე-საბურთალო, საბურთალო, ბუდაპეშტის ქ.</t>
         </is>
       </c>
     </row>
@@ -786,32 +786,32 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2150002₾</t>
+          <t>765000₾</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>75 კვ.მ.</t>
+          <t>177 კვ.მ.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>7/8</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>4/4</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>თბილისი, ტერევენკოს ქ.</t>
+          <t>თბილისი, ვაკე-საბურთალო, საბურთალო, მიცკევიჩის ქ.</t>
         </is>
       </c>
     </row>
@@ -821,17 +821,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2890001₾</t>
+          <t>305000₾</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>145 კვ.მ.</t>
+          <t>69 კვ.მ.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3/8</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -841,12 +841,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>9/14</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>თბილისი, ვაკე-საბურთალო, საბურთალო, ქავთარაძის ქ.</t>
+          <t>თბილისი, ვაკე-საბურთალო, საბურთალო, ს.ცინცაძის ქ.</t>
         </is>
       </c>
     </row>
@@ -856,17 +856,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2250003₾</t>
+          <t>156000₾</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>63 კვ.მ.</t>
+          <t>61 კვ.მ.</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -876,12 +876,12 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>7/8</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>თბილისი</t>
+          <t>3/8</t>
         </is>
       </c>
     </row>
@@ -891,32 +891,32 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1970004₾</t>
+          <t>5275004₾</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>46 კვ.მ.</t>
+          <t>123 კვ.მ.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>5/7</t>
+          <t>5/11</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>თბილისი</t>
+          <t>თბილისი, ვაკე-საბურთალო, საბურთალო</t>
         </is>
       </c>
     </row>
@@ -926,17 +926,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1490002₾</t>
+          <t>2435003₾</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>70 კვ.მ.</t>
+          <t>76 კვ.მ.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>15/16</t>
+          <t>1/5</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -951,7 +951,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>თბილისი, გიბრონიძის ქ.</t>
+          <t>თბილისი, ვაკე-საბურთალო, საბურთალო, ვაჟა-ფშაველას გამზ.</t>
         </is>
       </c>
     </row>
@@ -961,17 +961,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>8220005₾</t>
+          <t>205000₾</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>140 კვ.მ.</t>
+          <t>84 კვ.მ.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>7/16</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -981,12 +981,12 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>5/6</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>თბილისი, ძველი თბილისი, კრწანისი, გორგასლის ქ.</t>
+          <t>თბილისი, დიდუბე-ჩუღურეთი, დიღმის მასივი</t>
         </is>
       </c>
     </row>

</xml_diff>